<commit_message>
subtract presumed mean from input
</commit_message>
<xml_diff>
--- a/KerasTrainImagenet/train_v50.dropout.results.xlsx
+++ b/KerasTrainImagenet/train_v50.dropout.results.xlsx
@@ -912,7 +912,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H5"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2626,7 +2626,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O34">
-    <sortState ref="A5:O34">
+    <sortState ref="A2:O34">
       <sortCondition ref="N1:N34"/>
     </sortState>
   </autoFilter>

</xml_diff>